<commit_message>
added the possibility to create worksheet from stream template
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Other/StyleReferenceFiles/Named/output.xlsx
+++ b/ClosedXML_Tests/Resource/Other/StyleReferenceFiles/Named/output.xlsx
@@ -1,37 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\new temp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9811CE-7D79-4B63-94AA-2CDF6C2C8103}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="4695" yWindow="1935" windowWidth="24135" windowHeight="11385" firstSheet="0" activeTab="0" xr2:uid="{D7102381-98E9-4F3A-8A8D-52A0E4FB5801}"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <x:sheet name="Style Font" sheetId="5" r:id="rId5"/>
-    <x:sheet name="New sheet" sheetId="6" r:id="rId6"/>
+    <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Style Font" sheetId="3" r:id="rId3"/>
+    <x:sheet name="New sheet" sheetId="4" r:id="rId4"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="191029"/>
-  <x:extLst>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </x:ext>
-    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </x:ext>
-  </x:extLst>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
@@ -68,12 +48,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="11" x14ac:knownFonts="1">
-    <x:font>
+  <x:fonts count="11">
+    <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Century Gothic"/>
@@ -81,6 +62,40 @@
       <x:scheme val="minor"/>
     </x:font>
     <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF9C0006"/>
+      <x:name val="Century Gothic"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF006100"/>
+      <x:name val="Century Gothic"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="15"/>
+      <x:color theme="3"/>
+      <x:name val="Century Gothic"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF9C5700"/>
+      <x:name val="Century Gothic"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="18"/>
       <x:color theme="3"/>
       <x:name val="Century Gothic"/>
@@ -89,35 +104,7 @@
     </x:font>
     <x:font>
       <x:b/>
-      <x:sz val="15"/>
-      <x:color theme="3"/>
-      <x:name val="Century Gothic"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF006100"/>
-      <x:name val="Century Gothic"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF9C0006"/>
-      <x:name val="Century Gothic"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF9C5700"/>
-      <x:name val="Century Gothic"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:b/>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Century Gothic"/>
@@ -125,25 +112,28 @@
       <x:scheme val="minor"/>
     </x:font>
     <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Algerian"/>
       <x:family val="5"/>
     </x:font>
     <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Angsana New"/>
       <x:family val="1"/>
-      <x:charset val="222"/>
-    </x:font>
-    <x:font>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Arial Black"/>
       <x:family val="2"/>
     </x:font>
     <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Agency FB"/>
@@ -159,12 +149,12 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFC6EFCE"/>
+        <x:fgColor rgb="FFFFC7CE"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFFFC7CE"/>
+        <x:fgColor rgb="FFC6EFCE"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
@@ -174,55 +164,80 @@
     </x:fill>
   </x:fills>
   <x:borders count="3">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
       <x:bottom style="thick">
         <x:color theme="4"/>
       </x:bottom>
-      <x:diagonal/>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
-    <x:border>
-      <x:left/>
-      <x:right/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
       <x:top style="thin">
         <x:color theme="4"/>
       </x:top>
       <x:bottom style="double">
         <x:color theme="4"/>
       </x:bottom>
-      <x:diagonal/>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="16">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <x:xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <x:xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <x:xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+  <x:cellStyleXfs count="11">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -243,58 +258,61 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="17">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6"/>
-    <x:xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="4"/>
-    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3"/>
-    <x:xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5"/>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="7">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="8">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="9">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="10">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="11">
+  <x:cellXfs count="11">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
   <x:cellStyles count="7">
-    <x:cellStyle name="Bad" xfId="7" builtinId="27"/>
-    <x:cellStyle name="Good" xfId="8" builtinId="26"/>
-    <x:cellStyle name="Heading 1" xfId="9" builtinId="16"/>
-    <x:cellStyle name="Neutral" xfId="10" builtinId="28"/>
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <x:cellStyle name="Title" xfId="1" builtinId="15"/>
-    <x:cellStyle name="Total" xfId="11" builtinId="25"/>
+    <x:cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <x:cellStyle name="Good" xfId="2" builtinId="26"/>
+    <x:cellStyle name="Heading 1" xfId="3" builtinId="16"/>
+    <x:cellStyle name="Neutral" xfId="4" builtinId="28"/>
+    <x:cellStyle name="Title" xfId="5" builtinId="15"/>
+    <x:cellStyle name="Total" xfId="6" builtinId="25"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -341,7 +359,7 @@
     </a:clrScheme>
     <a:fontScheme name="Century Gothic">
       <a:majorFont>
-        <a:latin typeface="Century Gothic" panose="020F0302020204030204"/>
+        <a:latin typeface="Century Gothic"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="メイリオ"/>
@@ -376,7 +394,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Century Gothic" panose="020F0302020204030204"/>
+        <a:latin typeface="Century Gothic"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="メイリオ"/>
@@ -420,147 +438,171 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{E6975356-2C80-43F4-B9B6-30FA8187E32D}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -570,70 +612,69 @@
       <x:selection activeCell="H10" sqref="H10"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr defaultRowHeight="16.5"/>
   <x:cols>
     <x:col min="1" max="1" width="10.875" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="9.140625" style="0" customWidth="1"/>
     <x:col min="3" max="5" width="10.75" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <x:row r="1" spans="1:8">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <x:row r="2" spans="1:8">
       <x:c r="A2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:8" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <x:c r="A3" s="14" t="s">
+    <x:row r="3" spans="1:8" customFormat="1" ht="20.25" customHeight="1">
+      <x:c r="A3" s="3" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:8" customFormat="1" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <x:c r="A4" s="2" t="s">
+    <x:row r="4" spans="1:8" customFormat="1" ht="24.75" customHeight="1">
+      <x:c r="A4" s="5" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:8" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <x:c r="A5" s="16" t="s">
+    <x:row r="5" spans="1:8" customFormat="1" ht="17.25" customHeight="1">
+      <x:c r="A5" s="6" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:8" customFormat="1" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <x:c r="A6" s="12" t="s">
+    <x:row r="6" spans="1:8" customFormat="1" ht="17.25" customHeight="1">
+      <x:c r="A6" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <x:c r="A7" s="13" t="s">
+    <x:row r="7" spans="1:8">
+      <x:c r="A7" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <x:c r="A8" s="15" t="s">
+    <x:row r="8" spans="1:8">
+      <x:c r="A8" s="4" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C8" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:8" x14ac:dyDescent="0.3"/>
-    <x:row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <x:c r="H10" s="9" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <x:c r="F12" s="10" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <x:c r="E13" s="11" t="s"/>
+    <x:row r="10" spans="1:8">
+      <x:c r="H10" s="8" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:8" customFormat="1" ht="18.75" customHeight="1">
+      <x:c r="F12" s="9" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="E13" s="10" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" horizontalDpi="300" verticalDpi="300"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
@@ -651,7 +692,7 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="2" spans="1:2">
-      <x:c r="B2" s="12" t="s">
+      <x:c r="B2" s="1" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
fix bug when cell values are parsed even if cell numberformat is text
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Other/StyleReferenceFiles/Named/output.xlsx
+++ b/ClosedXML_Tests/Resource/Other/StyleReferenceFiles/Named/output.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <x:si>
     <x:t>sdasdada</x:t>
   </x:si>
@@ -40,6 +40,9 @@
   </x:si>
   <x:si>
     <x:t>afsfsdfsdfds</x:t>
+  </x:si>
+  <x:si>
+    <x:t>String</x:t>
   </x:si>
   <x:si>
     <x:t>Bold</x:t>
@@ -52,7 +55,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="11">
+  <x:fonts count="12">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -93,6 +96,13 @@
       <x:name val="Century Gothic"/>
       <x:family val="2"/>
       <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
@@ -237,28 +247,29 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="11">
+  <x:cellXfs count="13">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -279,15 +290,15 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="5">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="7">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -295,7 +306,11 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="5">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="5">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -303,15 +318,20 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellXfs>
-  <x:cellStyles count="7">
+  <x:cellStyles count="8">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
     <x:cellStyle name="Bad" xfId="1" builtinId="27"/>
     <x:cellStyle name="Good" xfId="2" builtinId="26"/>
     <x:cellStyle name="Heading 1" xfId="3" builtinId="16"/>
     <x:cellStyle name="Neutral" xfId="4" builtinId="28"/>
-    <x:cellStyle name="Title" xfId="5" builtinId="15"/>
-    <x:cellStyle name="Total" xfId="6" builtinId="25"/>
+    <x:cellStyle name="String" xfId="5"/>
+    <x:cellStyle name="Title" xfId="6" builtinId="15"/>
+    <x:cellStyle name="Total" xfId="7" builtinId="25"/>
   </x:cellStyles>
 </x:styleSheet>
 </file>
@@ -609,7 +629,7 @@
   <x:dimension ref="A1:H13"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="H10" sqref="H10"/>
+      <x:selection activeCell="A9" sqref="A9"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="16.5"/>
@@ -635,12 +655,12 @@
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8" customFormat="1" ht="24.75" customHeight="1">
-      <x:c r="A4" s="5" t="s">
+      <x:c r="A4" s="6" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8" customFormat="1" ht="17.25" customHeight="1">
-      <x:c r="A5" s="6" t="s">
+      <x:c r="A5" s="7" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
@@ -658,18 +678,23 @@
       <x:c r="A8" s="4" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C8" s="7" t="s">
+      <x:c r="C8" s="8" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
+    <x:row r="9" spans="1:8">
+      <x:c r="A9" s="9" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
     <x:row r="10" spans="1:8">
-      <x:c r="H10" s="8" t="s"/>
+      <x:c r="H10" s="10" t="s"/>
     </x:row>
     <x:row r="12" spans="1:8" customFormat="1" ht="18.75" customHeight="1">
-      <x:c r="F12" s="9" t="s"/>
+      <x:c r="F12" s="11" t="s"/>
     </x:row>
     <x:row r="13" spans="1:8">
-      <x:c r="E13" s="10" t="s"/>
+      <x:c r="E13" s="12" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -693,7 +718,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:2">
       <x:c r="B2" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>